<commit_message>
Solved JT problem; had to do with unequal weights in TRUTH sheet
Cause me much grief
</commit_message>
<xml_diff>
--- a/extdata/JT.xlsx
+++ b/extdata/JT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{523A73ED-804D-4A43-BBE8-7FA7803C187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D403C9-7104-AE47-BC0F-738B31A90CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19400" yWindow="8080" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{7057EA57-9FDF-894F-A8B2-5EE70FCCC0D4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="NL" sheetId="2" r:id="rId2"/>
     <sheet name="TRUTH" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25138,7 +25138,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C105"/>
+      <selection activeCell="C2" sqref="C2:C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25162,7 +25162,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -25173,7 +25173,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -25184,7 +25184,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -25195,7 +25195,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.83313091922005578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -25206,7 +25206,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>0.16756545961002783</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -25217,7 +25217,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.66536825473991246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -25228,7 +25228,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.33463174526008754</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -25239,7 +25239,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -25250,7 +25250,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -25261,7 +25261,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -25272,7 +25272,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -25283,7 +25283,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -25294,7 +25294,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -25305,7 +25305,7 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.8148596794235563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -25316,7 +25316,7 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0.18514032057644364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -25327,7 +25327,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -25338,7 +25338,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -25349,7 +25349,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -25360,7 +25360,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.28423228134424816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -25371,7 +25371,7 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>0.38606069582076685</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -25382,7 +25382,7 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.32970702283498488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -25393,7 +25393,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -25404,7 +25404,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -25415,7 +25415,7 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -25426,7 +25426,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -25437,7 +25437,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -25448,7 +25448,7 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -25459,7 +25459,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -25470,7 +25470,7 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -25481,7 +25481,7 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -25492,7 +25492,7 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -25503,7 +25503,7 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -25514,7 +25514,7 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -25525,7 +25525,7 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0.63615124228412134</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -25536,7 +25536,7 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>0.36384875771587866</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -25547,7 +25547,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -25558,7 +25558,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -25569,7 +25569,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -25580,7 +25580,7 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>0.7195696337408084</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -25591,7 +25591,7 @@
         <v>2</v>
       </c>
       <c r="C41">
-        <v>0.2804303662591916</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -25602,7 +25602,7 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -25613,7 +25613,7 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -25624,7 +25624,7 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <v>0.54880469718295066</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -25635,7 +25635,7 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <v>0.45119530281704934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -25646,7 +25646,7 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -25657,7 +25657,7 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -25668,7 +25668,7 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>0.39761410986658507</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -25679,7 +25679,7 @@
         <v>2</v>
       </c>
       <c r="C49">
-        <v>0.38261927061432011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -25690,7 +25690,7 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>0.21976661951909479</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -25701,7 +25701,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>0.25614983728355645</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -25712,7 +25712,7 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>0.74321503131524003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -25723,7 +25723,7 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -25734,7 +25734,7 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -25745,7 +25745,7 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>0.79651097565536078</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -25756,7 +25756,7 @@
         <v>2</v>
       </c>
       <c r="C56">
-        <v>0.20348902434463934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -25767,7 +25767,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -25778,7 +25778,7 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -25789,7 +25789,7 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -25800,7 +25800,7 @@
         <v>1</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>